<commit_message>
added partial fxml functionality
</commit_message>
<xml_diff>
--- a/my-app/src/main/resources/com/mycompany/model/InvoiceTemplate.xlsx
+++ b/my-app/src/main/resources/com/mycompany/model/InvoiceTemplate.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr codeName="ThisWorkbook" checkCompatibility="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremychow/personal-projects/InvoiceSystem/my-app/src/main/resources/com/mycompany/model/"/>
     </mc:Choice>
@@ -1888,7 +1888,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tooltip="Select to navigate to Customers worksheet"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{74092F0A-1B54-4027-B0EC-248D38E21E12}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74092F0A-1B54-4027-B0EC-248D38E21E12}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2007,7 +2007,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tooltip="Select to navigate to Commercial Invoice worksheet"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A369B219-35C8-4A3B-AB52-F207ECE6F82D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A369B219-35C8-4A3B-AB52-F207ECE6F82D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2441,15 +2441,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.6640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.6640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.1640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.6640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="18.83203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="2.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="22.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="2.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="15.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="25.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="27.1640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="15.6640625" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" style="1" width="18.83203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="17.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="2.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="22.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -2624,8 +2624,8 @@
       <c r="E9" s="39">
         <v>130</v>
       </c>
-      <c r="F9" s="40">
-        <v>0</v>
+      <c r="F9" s="40" t="n">
+        <v>0.0</v>
       </c>
       <c r="G9" s="40"/>
       <c r="H9" s="41">
@@ -2643,8 +2643,8 @@
       <c r="E10" s="39">
         <v>120</v>
       </c>
-      <c r="F10" s="40">
-        <v>0</v>
+      <c r="F10" s="40" t="n">
+        <v>0.0</v>
       </c>
       <c r="G10" s="40"/>
       <c r="H10" s="41">
@@ -2917,16 +2917,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="21.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="25.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.83203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="22.5" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="2.6640625" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="21.6640625" collapsed="true"/>
+    <col min="4" max="6" customWidth="true" width="25.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.83203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="22.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added model, more ui pages, better encapsulation
</commit_message>
<xml_diff>
--- a/my-app/src/main/resources/com/mycompany/model/InvoiceTemplate.xlsx
+++ b/my-app/src/main/resources/com/mycompany/model/InvoiceTemplate.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="301">
   <si>
     <t>Bill To:</t>
   </si>
@@ -933,6 +933,24 @@
   </si>
   <si>
     <t>dsad</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Lovpop</t>
+  </si>
+  <si>
+    <t>Fun</t>
+  </si>
+  <si>
+    <t>Boozipop</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -2618,16 +2636,20 @@
         <v>43665</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="39">
-        <v>130</v>
+        <v>296</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>296</v>
+      </c>
+      <c r="E9" s="39" t="n">
+        <v>0.0</v>
       </c>
       <c r="F9" s="40" t="n">
         <v>0.0</v>
       </c>
-      <c r="G9" s="40"/>
+      <c r="G9" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="H9" s="41">
         <f>(InvoiceItems[[#This Row],[Unit Price]]-InvoiceItems[[#This Row],[Unit Discount]])*InvoiceItems[[#This Row],[Qty]]</f>
         <v>0</v>
@@ -2637,16 +2659,20 @@
     <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="38"/>
       <c r="C10" s="36" t="s">
-        <v>294</v>
-      </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="39">
-        <v>120</v>
+        <v>296</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>296</v>
+      </c>
+      <c r="E10" s="39" t="n">
+        <v>0.0</v>
       </c>
       <c r="F10" s="40" t="n">
         <v>0.0</v>
       </c>
-      <c r="G10" s="40"/>
+      <c r="G10" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="H10" s="41">
         <f>(InvoiceItems[[#This Row],[Unit Price]]-InvoiceItems[[#This Row],[Unit Discount]])*InvoiceItems[[#This Row],[Qty]]</f>
         <v>0</v>
@@ -2655,11 +2681,21 @@
     </row>
     <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="38"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
+      <c r="C11" s="36" t="s">
+        <v>296</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>296</v>
+      </c>
+      <c r="E11" s="39" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F11" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G11" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="H11" s="41">
         <f>(InvoiceItems[[#This Row],[Unit Price]]-InvoiceItems[[#This Row],[Unit Discount]])*InvoiceItems[[#This Row],[Qty]]</f>
         <v>0</v>
@@ -2668,11 +2704,21 @@
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="38"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
+      <c r="C12" s="36" t="s">
+        <v>296</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>296</v>
+      </c>
+      <c r="E12" s="39" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F12" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G12" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="H12" s="41">
         <f>(InvoiceItems[[#This Row],[Unit Price]]-InvoiceItems[[#This Row],[Unit Discount]])*InvoiceItems[[#This Row],[Qty]]</f>
         <v>0</v>
@@ -2681,11 +2727,21 @@
     </row>
     <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="38"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
+      <c r="C13" s="36" t="s">
+        <v>296</v>
+      </c>
+      <c r="D13" s="36" t="s">
+        <v>296</v>
+      </c>
+      <c r="E13" s="39" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F13" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G13" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="H13" s="41">
         <f>(InvoiceItems[[#This Row],[Unit Price]]-InvoiceItems[[#This Row],[Unit Discount]])*InvoiceItems[[#This Row],[Qty]]</f>
         <v>0</v>
@@ -2694,11 +2750,21 @@
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="38"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
+      <c r="C14" s="36" t="s">
+        <v>296</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>296</v>
+      </c>
+      <c r="E14" s="39" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F14" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G14" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="H14" s="41">
         <f>(InvoiceItems[[#This Row],[Unit Price]]-InvoiceItems[[#This Row],[Unit Discount]])*InvoiceItems[[#This Row],[Qty]]</f>
         <v>0</v>

</xml_diff>